<commit_message>
Updates on egg tube data.
</commit_message>
<xml_diff>
--- a/prelims/data/egg_tube_data.xlsx
+++ b/prelims/data/egg_tube_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anastasiabernat/Desktop/git_repositories/extreme-flight-trials/prelims/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B0EF45-33B5-8549-BB2C-31723C55E7C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50FCFDD-0D21-8D4A-A39E-94665AB505C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" xr2:uid="{CE040209-3C16-F54B-BD28-83BB5606938B}"/>
+    <workbookView xWindow="640" yWindow="560" windowWidth="27280" windowHeight="16620" xr2:uid="{CE040209-3C16-F54B-BD28-83BB5606938B}"/>
   </bookViews>
   <sheets>
     <sheet name="egg_tube_data3" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4270" uniqueCount="68">
   <si>
     <t>gen1_ID</t>
   </si>
@@ -214,6 +214,21 @@
   </si>
   <si>
     <t>9.23.11</t>
+  </si>
+  <si>
+    <t>10.14.21</t>
+  </si>
+  <si>
+    <t>10.9-10.11</t>
+  </si>
+  <si>
+    <t>10.13.21</t>
+  </si>
+  <si>
+    <t>10.11.21</t>
+  </si>
+  <si>
+    <t>10.12.21</t>
   </si>
 </sst>
 </file>
@@ -654,8 +669,8 @@
   <dimension ref="A1:L1271"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A726" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E705" sqref="E705"/>
+      <pane ySplit="1" topLeftCell="A732" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H763" sqref="H763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2093,7 +2108,9 @@
       <c r="E49" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="F49" s="6"/>
+      <c r="F49" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G49" s="11" t="s">
         <v>17</v>
       </c>
@@ -10214,13 +10231,19 @@
       <c r="D336" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E336" s="6"/>
+      <c r="E336" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F336" s="6"/>
       <c r="G336" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H336" s="6"/>
-      <c r="I336" s="6"/>
+      <c r="H336" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I336" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J336" s="6" t="s">
         <v>30</v>
       </c>
@@ -11806,17 +11829,25 @@
       <c r="D392" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E392" s="6"/>
+      <c r="E392" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F392" s="6"/>
       <c r="G392" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H392" s="6"/>
-      <c r="I392" s="6"/>
+      <c r="H392" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I392" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J392" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K392" s="6"/>
+      <c r="K392" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="393" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A393" s="6">
@@ -13121,7 +13152,9 @@
       <c r="E438" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="F438" s="6"/>
+      <c r="F438" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="G438" s="11" t="s">
         <v>18</v>
       </c>
@@ -13303,12 +13336,18 @@
         <v>22</v>
       </c>
       <c r="E444" s="6"/>
-      <c r="F444" s="6"/>
+      <c r="F444" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="G444" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H444" s="6"/>
-      <c r="I444" s="6"/>
+      <c r="H444" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I444" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J444" s="6" t="s">
         <v>30</v>
       </c>
@@ -15999,7 +16038,9 @@
         <v>24</v>
       </c>
       <c r="E543" s="6"/>
-      <c r="F543" s="6"/>
+      <c r="F543" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="G543" s="11" t="s">
         <v>18</v>
       </c>
@@ -16047,7 +16088,9 @@
         <v>24</v>
       </c>
       <c r="E545" s="6"/>
-      <c r="F545" s="6"/>
+      <c r="F545" s="6" t="s">
+        <v>54</v>
+      </c>
       <c r="G545" s="11" t="s">
         <v>18</v>
       </c>
@@ -16102,13 +16145,19 @@
       <c r="D547" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E547" s="6"/>
+      <c r="E547" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="F547" s="6"/>
       <c r="G547" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H547" s="6"/>
-      <c r="I547" s="6"/>
+      <c r="H547" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I547" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J547" s="6" t="s">
         <v>30</v>
       </c>
@@ -17028,19 +17077,27 @@
       <c r="D579" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E579" s="6"/>
+      <c r="E579" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F579" s="6" t="s">
         <v>27</v>
       </c>
       <c r="G579" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H579" s="6"/>
-      <c r="I579" s="6"/>
+      <c r="H579" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I579" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J579" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K579" s="6"/>
+      <c r="K579" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="580" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A580" s="6">
@@ -17592,17 +17649,25 @@
       <c r="D601" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E601" s="6"/>
+      <c r="E601" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F601" s="6"/>
       <c r="G601" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H601" s="6"/>
-      <c r="I601" s="6"/>
+      <c r="H601" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I601" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J601" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K601" s="6"/>
+      <c r="K601" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="602" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A602" s="6">
@@ -17735,17 +17800,25 @@
       <c r="D606" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E606" s="6"/>
+      <c r="E606" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F606" s="6"/>
       <c r="G606" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H606" s="6"/>
-      <c r="I606" s="6"/>
+      <c r="H606" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I606" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J606" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K606" s="6"/>
+      <c r="K606" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="607" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A607" s="6">
@@ -18095,17 +18168,25 @@
       <c r="D618" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E618" s="6"/>
+      <c r="E618" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F618" s="6"/>
       <c r="G618" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H618" s="6"/>
-      <c r="I618" s="6"/>
+      <c r="H618" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I618" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J618" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K618" s="6"/>
+      <c r="K618" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="619" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A619" s="6">
@@ -18120,17 +18201,25 @@
       <c r="D619" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E619" s="6"/>
+      <c r="E619" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F619" s="6"/>
       <c r="G619" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H619" s="6"/>
-      <c r="I619" s="6"/>
+      <c r="H619" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I619" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J619" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K619" s="6"/>
+      <c r="K619" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="620" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A620" s="6">
@@ -18172,13 +18261,19 @@
       <c r="D621" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E621" s="6"/>
+      <c r="E621" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F621" s="6"/>
       <c r="G621" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H621" s="6"/>
-      <c r="I621" s="6"/>
+      <c r="H621" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I621" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J621" s="11" t="s">
         <v>30</v>
       </c>
@@ -18220,17 +18315,25 @@
       <c r="D623" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E623" s="6"/>
+      <c r="E623" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F623" s="6"/>
       <c r="G623" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H623" s="6"/>
-      <c r="I623" s="6"/>
+      <c r="H623" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I623" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J623" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K623" s="6"/>
+      <c r="K623" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="624" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A624" s="6">
@@ -18245,13 +18348,19 @@
       <c r="D624" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E624" s="6"/>
+      <c r="E624" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F624" s="6"/>
       <c r="G624" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H624" s="6"/>
-      <c r="I624" s="6"/>
+      <c r="H624" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I624" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J624" s="11" t="s">
         <v>30</v>
       </c>
@@ -18639,17 +18748,25 @@
       <c r="D638" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E638" s="6"/>
+      <c r="E638" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F638" s="6"/>
       <c r="G638" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H638" s="6"/>
-      <c r="I638" s="6"/>
+      <c r="H638" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I638" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J638" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K638" s="6"/>
+      <c r="K638" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="639" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A639" s="6">
@@ -18664,17 +18781,25 @@
       <c r="D639" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E639" s="6"/>
+      <c r="E639" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F639" s="6"/>
       <c r="G639" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H639" s="6"/>
-      <c r="I639" s="6"/>
+      <c r="H639" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I639" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J639" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K639" s="6"/>
+      <c r="K639" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="640" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A640" s="6">
@@ -18689,13 +18814,19 @@
       <c r="D640" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E640" s="6"/>
+      <c r="E640" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F640" s="6"/>
       <c r="G640" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H640" s="6"/>
-      <c r="I640" s="6"/>
+      <c r="H640" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I640" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J640" s="6" t="s">
         <v>30</v>
       </c>
@@ -18870,13 +19001,19 @@
       <c r="D647" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E647" s="6"/>
+      <c r="E647" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F647" s="6"/>
       <c r="G647" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H647" s="6"/>
-      <c r="I647" s="6"/>
+      <c r="H647" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I647" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J647" s="6" t="s">
         <v>30</v>
       </c>
@@ -18967,7 +19104,9 @@
         <v>41</v>
       </c>
       <c r="E651" s="6"/>
-      <c r="F651" s="6"/>
+      <c r="F651" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="G651" s="11" t="s">
         <v>18</v>
       </c>
@@ -19015,7 +19154,9 @@
         <v>40</v>
       </c>
       <c r="E653" s="6"/>
-      <c r="F653" s="6"/>
+      <c r="F653" s="6" t="s">
+        <v>51</v>
+      </c>
       <c r="G653" s="11" t="s">
         <v>18</v>
       </c>
@@ -19230,17 +19371,25 @@
       <c r="D661" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E661" s="6"/>
+      <c r="E661" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F661" s="6"/>
       <c r="G661" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H661" s="6"/>
-      <c r="I661" s="6"/>
+      <c r="H661" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I661" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J661" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K661" s="6"/>
+      <c r="K661" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="662" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A662" s="6">
@@ -19286,13 +19435,19 @@
       <c r="D663" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E663" s="6"/>
+      <c r="E663" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="F663" s="6"/>
       <c r="G663" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H663" s="6"/>
-      <c r="I663" s="6"/>
+      <c r="H663" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I663" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J663" s="6" t="s">
         <v>30</v>
       </c>
@@ -19391,7 +19546,9 @@
         <v>40</v>
       </c>
       <c r="E667" s="6"/>
-      <c r="F667" s="6"/>
+      <c r="F667" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="G667" s="11" t="s">
         <v>18</v>
       </c>
@@ -19413,15 +19570,23 @@
         <v>38</v>
       </c>
       <c r="D668" s="6"/>
-      <c r="E668" s="6"/>
+      <c r="E668" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F668" s="6"/>
       <c r="G668" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H668" s="6"/>
-      <c r="I668" s="6"/>
+      <c r="H668" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I668" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J668" s="6"/>
-      <c r="K668" s="6"/>
+      <c r="K668" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="669" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A669" s="6">
@@ -19434,15 +19599,23 @@
         <v>38</v>
       </c>
       <c r="D669" s="6"/>
-      <c r="E669" s="6"/>
+      <c r="E669" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F669" s="6"/>
       <c r="G669" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H669" s="6"/>
-      <c r="I669" s="6"/>
+      <c r="H669" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I669" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J669" s="6"/>
-      <c r="K669" s="6"/>
+      <c r="K669" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="670" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A670" s="6">
@@ -19457,17 +19630,25 @@
       <c r="D670" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E670" s="6"/>
+      <c r="E670" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F670" s="6"/>
       <c r="G670" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H670" s="6"/>
-      <c r="I670" s="6"/>
+      <c r="H670" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I670" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J670" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K670" s="6"/>
+      <c r="K670" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="671" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A671" s="6">
@@ -19588,7 +19769,9 @@
       <c r="D675" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E675" s="6"/>
+      <c r="E675" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F675" s="6"/>
       <c r="G675" s="11" t="s">
         <v>18</v>
@@ -19598,7 +19781,9 @@
       <c r="J675" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K675" s="6"/>
+      <c r="K675" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="676" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A676" s="6">
@@ -19679,13 +19864,19 @@
       <c r="D678" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="E678" s="6"/>
+      <c r="E678" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F678" s="6"/>
       <c r="G678" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H678" s="6"/>
-      <c r="I678" s="6"/>
+      <c r="H678" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I678" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J678" s="6"/>
       <c r="K678" s="6"/>
     </row>
@@ -19702,15 +19893,23 @@
       <c r="D679" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E679" s="6"/>
+      <c r="E679" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F679" s="6"/>
       <c r="G679" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H679" s="6"/>
-      <c r="I679" s="6"/>
+      <c r="H679" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I679" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J679" s="6"/>
-      <c r="K679" s="6"/>
+      <c r="K679" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="680" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A680" s="6">
@@ -19779,15 +19978,23 @@
       <c r="D682" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E682" s="6"/>
+      <c r="E682" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F682" s="6"/>
       <c r="G682" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H682" s="6"/>
-      <c r="I682" s="6"/>
+      <c r="H682" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I682" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J682" s="6"/>
-      <c r="K682" s="6"/>
+      <c r="K682" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="683" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A683" s="6">
@@ -19827,15 +20034,23 @@
       <c r="D684" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E684" s="8"/>
+      <c r="E684" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="F684" s="8"/>
       <c r="G684" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H684" s="8"/>
-      <c r="I684" s="8"/>
+      <c r="H684" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I684" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J684" s="8"/>
-      <c r="K684" s="8"/>
+      <c r="K684" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="685" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A685" s="9">
@@ -19894,17 +20109,25 @@
       <c r="D687" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E687" s="9"/>
+      <c r="E687" s="9" t="s">
+        <v>66</v>
+      </c>
       <c r="F687" s="9"/>
       <c r="G687" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="H687" s="9"/>
-      <c r="I687" s="9"/>
+      <c r="H687" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I687" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="J687" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="K687" s="9"/>
+      <c r="K687" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="688" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A688" s="6">
@@ -20097,17 +20320,25 @@
       <c r="D694" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E694" s="6"/>
+      <c r="E694" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F694" s="6"/>
       <c r="G694" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H694" s="6"/>
-      <c r="I694" s="6"/>
+      <c r="H694" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I694" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J694" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K694" s="6"/>
+      <c r="K694" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="695" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A695" s="6">
@@ -20184,13 +20415,19 @@
       <c r="D697" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E697" s="8"/>
+      <c r="E697" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="F697" s="8"/>
       <c r="G697" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="H697" s="8"/>
-      <c r="I697" s="8"/>
+      <c r="H697" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I697" s="8" t="s">
+        <v>30</v>
+      </c>
       <c r="J697" s="8" t="s">
         <v>30</v>
       </c>
@@ -20240,13 +20477,19 @@
       <c r="D699" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E699" s="6"/>
+      <c r="E699" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F699" s="6"/>
       <c r="G699" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H699" s="6"/>
-      <c r="I699" s="6"/>
+      <c r="H699" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I699" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J699" s="11" t="s">
         <v>30</v>
       </c>
@@ -20265,13 +20508,19 @@
       <c r="D700" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E700" s="6"/>
+      <c r="E700" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="F700" s="6"/>
       <c r="G700" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H700" s="6"/>
-      <c r="I700" s="6"/>
+      <c r="H700" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I700" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J700" s="11" t="s">
         <v>30</v>
       </c>
@@ -20290,13 +20539,19 @@
       <c r="D701" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E701" s="6"/>
+      <c r="E701" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="F701" s="6"/>
       <c r="G701" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="H701" s="6"/>
-      <c r="I701" s="6"/>
+      <c r="H701" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I701" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J701" s="11" t="s">
         <v>30</v>
       </c>
@@ -20346,13 +20601,19 @@
       <c r="D703" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="E703" s="8"/>
+      <c r="E703" s="8" t="s">
+        <v>65</v>
+      </c>
       <c r="F703" s="8"/>
       <c r="G703" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H703" s="8"/>
-      <c r="I703" s="8"/>
+      <c r="H703" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="I703" s="8" t="s">
+        <v>33</v>
+      </c>
       <c r="J703" s="12" t="s">
         <v>30</v>
       </c>
@@ -20755,17 +21016,25 @@
       <c r="D720" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E720" s="6"/>
+      <c r="E720" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F720" s="6"/>
       <c r="G720" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H720" s="6"/>
-      <c r="I720" s="6"/>
+      <c r="H720" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I720" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J720" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K720" s="6"/>
+      <c r="K720" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="721" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A721" s="6">
@@ -20803,17 +21072,25 @@
       <c r="D722" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E722" s="6"/>
+      <c r="E722" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F722" s="6"/>
       <c r="G722" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H722" s="6"/>
-      <c r="I722" s="6"/>
+      <c r="H722" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I722" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J722" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K722" s="6"/>
+      <c r="K722" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="723" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A723" s="6">
@@ -20829,7 +21106,9 @@
         <v>42</v>
       </c>
       <c r="E723" s="6"/>
-      <c r="F723" s="6"/>
+      <c r="F723" s="6" t="s">
+        <v>65</v>
+      </c>
       <c r="G723" s="11" t="s">
         <v>18</v>
       </c>
@@ -21247,13 +21526,19 @@
       <c r="D740" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E740" s="6"/>
+      <c r="E740" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F740" s="6"/>
       <c r="G740" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H740" s="6"/>
-      <c r="I740" s="6"/>
+      <c r="H740" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I740" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J740" s="6"/>
       <c r="K740" s="6"/>
     </row>
@@ -21270,15 +21555,23 @@
       <c r="D741" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E741" s="6"/>
+      <c r="E741" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F741" s="6"/>
       <c r="G741" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H741" s="6"/>
-      <c r="I741" s="6"/>
+      <c r="H741" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I741" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J741" s="6"/>
-      <c r="K741" s="6"/>
+      <c r="K741" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="742" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A742" s="6">
@@ -21293,15 +21586,23 @@
       <c r="D742" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E742" s="6"/>
+      <c r="E742" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F742" s="6"/>
       <c r="G742" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H742" s="6"/>
-      <c r="I742" s="6"/>
+      <c r="H742" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I742" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J742" s="6"/>
-      <c r="K742" s="6"/>
+      <c r="K742" s="6" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="743" spans="1:11" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A743" s="6">
@@ -21316,7 +21617,6 @@
       <c r="D743" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E743" s="6"/>
       <c r="F743" s="6"/>
       <c r="G743" s="11" t="s">
         <v>18</v>
@@ -21339,13 +21639,19 @@
       <c r="D744" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E744" s="6"/>
+      <c r="E744" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F744" s="6"/>
       <c r="G744" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H744" s="6"/>
-      <c r="I744" s="6"/>
+      <c r="H744" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I744" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J744" s="6"/>
       <c r="K744" s="6"/>
     </row>
@@ -21408,13 +21714,19 @@
       <c r="D747" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E747" s="6"/>
+      <c r="E747" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F747" s="6"/>
       <c r="G747" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H747" s="6"/>
-      <c r="I747" s="6"/>
+      <c r="H747" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I747" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="J747" s="6"/>
       <c r="K747" s="6"/>
     </row>
@@ -21454,13 +21766,19 @@
       <c r="D749" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E749" s="6"/>
+      <c r="E749" s="6" t="s">
+        <v>67</v>
+      </c>
       <c r="F749" s="6"/>
       <c r="G749" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H749" s="6"/>
-      <c r="I749" s="6"/>
+      <c r="H749" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I749" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J749" s="6"/>
       <c r="K749" s="6"/>
     </row>
@@ -21477,13 +21795,19 @@
       <c r="D750" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E750" s="6"/>
+      <c r="E750" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F750" s="6"/>
       <c r="G750" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H750" s="6"/>
-      <c r="I750" s="6"/>
+      <c r="H750" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I750" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J750" s="6"/>
       <c r="K750" s="6"/>
     </row>
@@ -21500,13 +21824,19 @@
       <c r="D751" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E751" s="6"/>
+      <c r="E751" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F751" s="6"/>
       <c r="G751" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H751" s="6"/>
-      <c r="I751" s="6"/>
+      <c r="H751" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I751" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J751" s="6"/>
       <c r="K751" s="6"/>
     </row>
@@ -21638,13 +21968,19 @@
       <c r="D757" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E757" s="6"/>
+      <c r="E757" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F757" s="6"/>
       <c r="G757" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H757" s="6"/>
-      <c r="I757" s="6"/>
+      <c r="H757" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I757" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J757" s="6"/>
       <c r="K757" s="6"/>
     </row>
@@ -21684,13 +22020,19 @@
       <c r="D759" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E759" s="6"/>
+      <c r="E759" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F759" s="6"/>
       <c r="G759" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H759" s="6"/>
-      <c r="I759" s="6"/>
+      <c r="H759" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I759" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J759" s="6"/>
       <c r="K759" s="6"/>
     </row>
@@ -21707,13 +22049,19 @@
       <c r="D760" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E760" s="6"/>
+      <c r="E760" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F760" s="6"/>
       <c r="G760" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H760" s="6"/>
-      <c r="I760" s="6"/>
+      <c r="H760" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I760" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J760" s="6"/>
       <c r="K760" s="6"/>
     </row>
@@ -21753,13 +22101,19 @@
       <c r="D762" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E762" s="6"/>
+      <c r="E762" s="6" t="s">
+        <v>63</v>
+      </c>
       <c r="F762" s="6"/>
       <c r="G762" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="H762" s="6"/>
-      <c r="I762" s="6"/>
+      <c r="H762" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I762" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="J762" s="6"/>
       <c r="K762" s="6"/>
     </row>

</xml_diff>